<commit_message>
started a build_iteminfo.py script
</commit_message>
<xml_diff>
--- a/Mob__DB_Editor.xlsx
+++ b/Mob__DB_Editor.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="132" windowWidth="8580" windowHeight="1104"/>
+    <workbookView xWindow="96" yWindow="132" windowWidth="8580" windowHeight="1140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mob_Db" sheetId="1" r:id="rId1"/>
     <sheet name="Codes" sheetId="2" r:id="rId2"/>
+    <sheet name="Mob_Skills" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="MD_AGGRESSIVE">Codes!$E$9</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="235">
   <si>
     <t>ID</t>
   </si>
@@ -637,6 +638,99 @@
   </si>
   <si>
     <t>Concat</t>
+  </si>
+  <si>
+    <t>Aquaring@AL_HEAL</t>
+  </si>
+  <si>
+    <t>attack</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>myhpltmaxrate</t>
+  </si>
+  <si>
+    <t>Aquaring@NPC_WATERATTACK</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>always</t>
+  </si>
+  <si>
+    <t>Aquaring@WZ_WATERBALL</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>MobID</t>
+  </si>
+  <si>
+    <t>Dummy value (info only)</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>SkillID</t>
+  </si>
+  <si>
+    <t>SkillLv</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>CastTime</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Cancelable</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Condition type</t>
+  </si>
+  <si>
+    <t>Condition value</t>
+  </si>
+  <si>
+    <t>val1</t>
+  </si>
+  <si>
+    <t>val2</t>
+  </si>
+  <si>
+    <t>val3</t>
+  </si>
+  <si>
+    <t>val4</t>
+  </si>
+  <si>
+    <t>val5</t>
+  </si>
+  <si>
+    <t>Emotion</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Waterball</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Water Attack</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2408,4 +2502,240 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L1" t="s">
+        <v>223</v>
+      </c>
+      <c r="M1" t="s">
+        <v>224</v>
+      </c>
+      <c r="N1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P1" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R1" t="s">
+        <v>229</v>
+      </c>
+      <c r="S1" t="s">
+        <v>230</v>
+      </c>
+      <c r="T1" t="s">
+        <v>231</v>
+      </c>
+      <c r="U1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2">
+        <v>3950</v>
+      </c>
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <f>10000*0.1</f>
+        <v>1000</v>
+      </c>
+      <c r="H2">
+        <f>2.5*1000</f>
+        <v>2500</v>
+      </c>
+      <c r="I2">
+        <f>1000*2.5</f>
+        <v>2500</v>
+      </c>
+      <c r="J2" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" t="s">
+        <v>206</v>
+      </c>
+      <c r="L2" t="s">
+        <v>207</v>
+      </c>
+      <c r="M2">
+        <v>25</v>
+      </c>
+      <c r="U2" t="str">
+        <f>B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;","&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;","&amp;M2&amp;","&amp;N2&amp;","&amp;O2&amp;","&amp;P2&amp;","&amp;Q2&amp;","&amp;R2&amp;","&amp;S2&amp;","&amp;T2</f>
+        <v>3950,Aquaring@AL_HEAL,attack,15,15,1000,2500,2500,no,self,myhpltmaxrate,25,,,,,,,</v>
+      </c>
+      <c r="V2" t="str">
+        <f>"Casts level "&amp;F2&amp;" "&amp;A2&amp;" at "&amp;G2/100&amp;"%"&amp;" on "&amp;PROPER(D2)&amp;"."</f>
+        <v>Casts level 15 Heal at 10% on Attack.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3">
+        <v>3950</v>
+      </c>
+      <c r="C3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3">
+        <v>184</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <f>10000*0.2</f>
+        <v>2000</v>
+      </c>
+      <c r="H3">
+        <f>0*1000</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>1000*5</f>
+        <v>5000</v>
+      </c>
+      <c r="J3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L3" t="s">
+        <v>210</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U4" si="0">B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3</f>
+        <v>3950,Aquaring@NPC_WATERATTACK,attack,184,5,2000,0,5000,no,target,always,0,,,,,,,</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V4" si="1">"Casts level "&amp;F3&amp;" "&amp;A3&amp;" at "&amp;G3/100&amp;"%"&amp;" on "&amp;PROPER(D3)&amp;"."</f>
+        <v>Casts level 5 Water Attack at 20% on Attack.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4">
+        <v>3950</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4">
+        <v>86</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <f>10000*0.03</f>
+        <v>300</v>
+      </c>
+      <c r="H4">
+        <f>2*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="I4">
+        <f>1000*0</f>
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>212</v>
+      </c>
+      <c r="K4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L4" t="s">
+        <v>210</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="0"/>
+        <v>3950,Aquaring@WZ_WATERBALL,attack,86,5,300,2000,0,no,target,always,0,,,,,,,</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="1"/>
+        <v>Casts level 5 Waterball at 3% on Attack.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>